<commit_message>
Corrected the Sucep_new file
Corrected the file and other functions associated with it
</commit_message>
<xml_diff>
--- a/Input/dados_teste/suscep_classes_new.xlsx
+++ b/Input/dados_teste/suscep_classes_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/febagnatori/Documents/GitHub/ScientificResearchAtibiotics/Output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/febagnatori/Documents/GitHub/ScientificResearchAtibiotics/Input/dados_teste/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1E3255-BF13-704A-A26D-077E122D10C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52F75AA-1F73-3840-B9F6-D7FDA4B79A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3220" yWindow="920" windowWidth="15080" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="1020" windowWidth="14880" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>0.053</t>
+  </si>
+  <si>
+    <t>0.125</t>
+  </si>
+  <si>
+    <t>0.250</t>
+  </si>
+  <si>
+    <t>0.500</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -96,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -108,6 +125,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,42 +430,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="C1" s="1">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1">
         <v>4</v>
       </c>
-      <c r="F1" s="1">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1">
+      <c r="I1" s="1">
         <v>8</v>
       </c>
-      <c r="H1" s="1">
-        <v>12</v>
-      </c>
-      <c r="I1" s="1">
+      <c r="J1" s="1">
         <v>16</v>
-      </c>
-      <c r="J1" s="1">
-        <v>25</v>
       </c>
       <c r="K1" s="1">
         <v>32</v>
@@ -467,10 +487,7 @@
       <c r="I2">
         <v>0</v>
       </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
+      <c r="J2">
         <v>2</v>
       </c>
     </row>
@@ -478,13 +495,10 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="K3">
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>2</v>
       </c>
     </row>
@@ -494,16 +508,25 @@
       </c>
       <c r="F4">
         <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="L5">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
         <v>2</v>
       </c>
     </row>
@@ -511,27 +534,21 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>2</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="C7">
-        <v>1</v>
+      <c r="G7">
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="M7">
         <v>2</v>
       </c>
     </row>
@@ -539,10 +556,13 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
         <v>2</v>
       </c>
     </row>
@@ -553,10 +573,10 @@
       <c r="E9">
         <v>0</v>
       </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
       <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="K9">
         <v>2</v>
       </c>
     </row>
@@ -565,12 +585,12 @@
         <v>8</v>
       </c>
       <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="I10">
         <v>1</v>
       </c>
       <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="L10">
         <v>2</v>
       </c>
     </row>
@@ -579,37 +599,34 @@
         <v>9</v>
       </c>
       <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>2</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>2</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="K13">
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
         <v>2</v>
       </c>
     </row>
@@ -617,38 +634,14 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="K16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>